<commit_message>
can now remove rows but it is weird
</commit_message>
<xml_diff>
--- a/PEATA/data/exports/tiktok_videos.xlsx
+++ b/PEATA/data/exports/tiktok_videos.xlsx
@@ -434,7 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>[{'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_description': '', 'hashtag_id': 3979591, 'hashtag_name': 'firewings'}, {'hashtag_description': '', 'hashtag_id': 47867, 'hashtag_name': 'chickenwing'}, {'hashtag_description': '', 'hashtag_id': 2556710, 'hashtag_name': 'familygames'}, {'hashtag_name': 'FamilyGameNight', 'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}]</t>
+          <t>[{'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_description': '', 'hashtag_id': 3979591, 'hashtag_name': 'firewings'}, {'hashtag_description': '', 'hashtag_id': 47867, 'hashtag_name': 'chickenwing'}, {'hashtag_description': '', 'hashtag_id': 2556710, 'hashtag_name': 'familygames'}, {'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421, 'hashtag_name': 'FamilyGameNight'}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}]</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -454,7 +454,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>252129</t>
+          <t>252133</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>{'content': '', 'sink': False, 'type': 0, 'vote': False, 'warn': False}</t>
+          <t>{'vote': False, 'warn': False, 'content': '', 'sink': False, 'type': 0}</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
@@ -499,7 +499,7 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>4314143</t>
+          <t>4314291</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
@@ -522,7 +522,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[{'hashtag_description': '', 'hashtag_id': 47867, 'hashtag_name': 'chickenwing'}, {'hashtag_description': '', 'hashtag_id': 2556710, 'hashtag_name': 'familygames'}, {'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421, 'hashtag_name': 'FamilyGameNight'}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}, {'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_description': '', 'hashtag_id': 3979591, 'hashtag_name': 'firewings'}]</t>
+          <t>[{'hashtag_name': 'xyzbca', 'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509}, {'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_name': 'firewings', 'hashtag_description': '', 'hashtag_id': 3979591}, {'hashtag_description': '', 'hashtag_id': 47867, 'hashtag_name': 'chickenwing'}, {'hashtag_id': 2556710, 'hashtag_name': 'familygames', 'hashtag_description': ''}, {'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421, 'hashtag_name': 'FamilyGameNight'}]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>71024</t>
+          <t>71028</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>{'type': 0, 'vote': False, 'warn': False, 'content': '', 'sink': False}</t>
+          <t>{'content': '', 'sink': False, 'type': 0, 'vote': False, 'warn': False}</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1719401</t>
+          <t>1719544</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">

</xml_diff>